<commit_message>
All files are added
</commit_message>
<xml_diff>
--- a/Learning Progress.xlsx
+++ b/Learning Progress.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Learning\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD497A4-9244-481F-85FA-F8A8C59C2989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,46 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t xml:space="preserve">Date </t>
+  </si>
+  <si>
+    <t>Time Spent</t>
+  </si>
+  <si>
+    <t>Topics Covered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File name </t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certifications </t>
+  </si>
+  <si>
+    <t>3-4 Hours</t>
+  </si>
+  <si>
+    <t>Git &amp; Github- Branching, Merging, Rebase and other basic commands</t>
+  </si>
+  <si>
+    <t>1)Installation and basic commands  2) Branching  3) auto email  4) Tags         5) Merging vs Rebase</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/certificate/UC-a8fc2a6b-4f1b-4ce1-9af5-921adb6fd73d/</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +93,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +378,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>45000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>